<commit_message>
#39 rearranged test cases
</commit_message>
<xml_diff>
--- a/SHS_D2_useCases.xlsx
+++ b/SHS_D2_useCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Defaut\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgekoutsaris/Desktop/UNIVERSITY/Concordia/SEMESTERS/FALL 2020/SOEN 343/SOEN 343 PROJECT/soen343_project_delivery1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{917A7170-A3E0-4910-BC2F-050C31A5F65A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A2B8D7-3A2F-BB41-B0A7-CC7686E350E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5797803E-4189-4FD0-96CB-DECF01A43E99}"/>
+    <workbookView xWindow="13660" yWindow="460" windowWidth="23260" windowHeight="16820" xr2:uid="{5797803E-4189-4FD0-96CB-DECF01A43E99}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -356,7 +356,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -657,18 +657,18 @@
   </sheetPr>
   <dimension ref="B2:C92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="132" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="61.109375" customWidth="1"/>
+    <col min="3" max="3" width="61.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
@@ -676,7 +676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -684,7 +684,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -692,7 +692,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -700,7 +700,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
@@ -708,7 +708,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" ht="48" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
         <v>4</v>
       </c>
@@ -716,7 +716,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
@@ -724,7 +724,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
@@ -732,7 +732,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
@@ -740,7 +740,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -748,7 +748,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -756,7 +756,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" ht="32" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
         <v>3</v>
       </c>
@@ -772,7 +772,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" ht="112" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
         <v>4</v>
       </c>
@@ -780,7 +780,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
@@ -788,7 +788,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>8</v>
       </c>
@@ -796,7 +796,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>24</v>
       </c>
@@ -804,7 +804,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>0</v>
       </c>
@@ -812,7 +812,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>1</v>
       </c>
@@ -820,7 +820,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" ht="48" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
         <v>2</v>
       </c>
@@ -828,7 +828,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
         <v>3</v>
       </c>
@@ -836,7 +836,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" ht="128" x14ac:dyDescent="0.2">
       <c r="B25" s="11" t="s">
         <v>4</v>
       </c>
@@ -844,7 +844,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" ht="32" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
@@ -852,7 +852,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
         <v>8</v>
       </c>
@@ -860,7 +860,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
@@ -868,7 +868,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
         <v>0</v>
       </c>
@@ -876,7 +876,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
         <v>1</v>
       </c>
@@ -884,7 +884,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3" ht="64" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
         <v>2</v>
       </c>
@@ -892,7 +892,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
         <v>3</v>
       </c>
@@ -900,7 +900,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3" ht="80" x14ac:dyDescent="0.2">
       <c r="B34" s="11" t="s">
         <v>4</v>
       </c>
@@ -908,7 +908,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B35" s="3" t="s">
         <v>5</v>
       </c>
@@ -916,7 +916,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:3" ht="32" x14ac:dyDescent="0.2">
       <c r="B36" s="3" t="s">
         <v>8</v>
       </c>
@@ -924,223 +924,223 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B41" s="13"/>
       <c r="C41" s="14"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B42" s="13"/>
       <c r="C42" s="15"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B43" s="16"/>
       <c r="C43" s="17"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" s="13"/>
       <c r="C49" s="13"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B50" s="13"/>
       <c r="C50" s="13"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B51" s="13"/>
       <c r="C51" s="13"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B52" s="16"/>
       <c r="C52" s="17"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B53" s="13"/>
       <c r="C53" s="13"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B55" s="13"/>
       <c r="C55" s="13"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B56" s="13"/>
       <c r="C56" s="13"/>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B57" s="13"/>
       <c r="C57" s="13"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B61" s="16"/>
       <c r="C61" s="17"/>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B63" s="13"/>
       <c r="C63" s="13"/>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B66" s="13"/>
       <c r="C66" s="13"/>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B67" s="13"/>
       <c r="C67" s="13"/>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B68" s="13"/>
       <c r="C68" s="13"/>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B69" s="13"/>
       <c r="C69" s="13"/>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B70" s="16"/>
       <c r="C70" s="17"/>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B71" s="13"/>
       <c r="C71" s="18"/>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B72" s="13"/>
       <c r="C72" s="13"/>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B73" s="13"/>
       <c r="C73" s="13"/>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B74" s="13"/>
       <c r="C74" s="13"/>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B76" s="13"/>
       <c r="C76" s="13"/>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B77" s="13"/>
       <c r="C77" s="13"/>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B78" s="13"/>
       <c r="C78" s="13"/>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B79" s="16"/>
       <c r="C79" s="17"/>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B80" s="13"/>
       <c r="C80" s="18"/>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B81" s="13"/>
       <c r="C81" s="13"/>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B82" s="13"/>
       <c r="C82" s="13"/>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B83" s="13"/>
       <c r="C83" s="13"/>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B84" s="13"/>
       <c r="C84" s="13"/>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B85" s="13"/>
       <c r="C85" s="13"/>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B87" s="13"/>
       <c r="C87" s="13"/>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B88" s="16"/>
       <c r="C88" s="17"/>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B89" s="13"/>
       <c r="C89" s="18"/>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B90" s="13"/>
       <c r="C90" s="13"/>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B92" s="13"/>
       <c r="C92" s="13"/>
     </row>

</xml_diff>